<commit_message>
P5: add sensor configurations
</commit_message>
<xml_diff>
--- a/virus_situations/Covera17_situations.xlsx
+++ b/virus_situations/Covera17_situations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="12525"/>
+    <workbookView windowWidth="21750" windowHeight="12525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -56,6 +56,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -65,6 +72,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -94,6 +108,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -102,25 +124,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -134,7 +142,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,44 +171,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,19 +200,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -224,37 +368,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,121 +380,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,11 +418,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -442,17 +448,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -474,11 +476,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,8 +486,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,142 +496,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -707,6 +707,1417 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr defTabSz="914400">
+              <a:defRPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>Corona virus </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.392708333333333"/>
+          <c:y val="0.0277777777777778"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Confirmed cases</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$2:$A$20</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0" c:formatCode="d\-mmm">
+                  <c:v>44631</c:v>
+                </c:pt>
+                <c:pt idx="1" c:formatCode="d\-mmm">
+                  <c:v>44632</c:v>
+                </c:pt>
+                <c:pt idx="2" c:formatCode="d\-mmm">
+                  <c:v>44633</c:v>
+                </c:pt>
+                <c:pt idx="3" c:formatCode="d\-mmm">
+                  <c:v>44634</c:v>
+                </c:pt>
+                <c:pt idx="4" c:formatCode="d\-mmm">
+                  <c:v>44635</c:v>
+                </c:pt>
+                <c:pt idx="5" c:formatCode="d\-mmm">
+                  <c:v>44636</c:v>
+                </c:pt>
+                <c:pt idx="6" c:formatCode="d\-mmm">
+                  <c:v>44637</c:v>
+                </c:pt>
+                <c:pt idx="7" c:formatCode="d\-mmm">
+                  <c:v>44638</c:v>
+                </c:pt>
+                <c:pt idx="8" c:formatCode="d\-mmm">
+                  <c:v>44639</c:v>
+                </c:pt>
+                <c:pt idx="9" c:formatCode="d\-mmm">
+                  <c:v>44640</c:v>
+                </c:pt>
+                <c:pt idx="10" c:formatCode="d\-mmm">
+                  <c:v>44641</c:v>
+                </c:pt>
+                <c:pt idx="11" c:formatCode="d\-mmm">
+                  <c:v>44642</c:v>
+                </c:pt>
+                <c:pt idx="12" c:formatCode="d\-mmm">
+                  <c:v>44643</c:v>
+                </c:pt>
+                <c:pt idx="13" c:formatCode="d\-mmm">
+                  <c:v>44644</c:v>
+                </c:pt>
+                <c:pt idx="14" c:formatCode="d\-mmm">
+                  <c:v>44645</c:v>
+                </c:pt>
+                <c:pt idx="15" c:formatCode="d\-mmm">
+                  <c:v>44646</c:v>
+                </c:pt>
+                <c:pt idx="16" c:formatCode="d\-mmm">
+                  <c:v>44647</c:v>
+                </c:pt>
+                <c:pt idx="17" c:formatCode="d\-mmm">
+                  <c:v>44648</c:v>
+                </c:pt>
+                <c:pt idx="18" c:formatCode="d\-mmm">
+                  <c:v>44649</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$2:$B$21</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$2:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>326</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Asymptomatic cases</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$2:$A$20</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0" c:formatCode="d\-mmm">
+                  <c:v>44631</c:v>
+                </c:pt>
+                <c:pt idx="1" c:formatCode="d\-mmm">
+                  <c:v>44632</c:v>
+                </c:pt>
+                <c:pt idx="2" c:formatCode="d\-mmm">
+                  <c:v>44633</c:v>
+                </c:pt>
+                <c:pt idx="3" c:formatCode="d\-mmm">
+                  <c:v>44634</c:v>
+                </c:pt>
+                <c:pt idx="4" c:formatCode="d\-mmm">
+                  <c:v>44635</c:v>
+                </c:pt>
+                <c:pt idx="5" c:formatCode="d\-mmm">
+                  <c:v>44636</c:v>
+                </c:pt>
+                <c:pt idx="6" c:formatCode="d\-mmm">
+                  <c:v>44637</c:v>
+                </c:pt>
+                <c:pt idx="7" c:formatCode="d\-mmm">
+                  <c:v>44638</c:v>
+                </c:pt>
+                <c:pt idx="8" c:formatCode="d\-mmm">
+                  <c:v>44639</c:v>
+                </c:pt>
+                <c:pt idx="9" c:formatCode="d\-mmm">
+                  <c:v>44640</c:v>
+                </c:pt>
+                <c:pt idx="10" c:formatCode="d\-mmm">
+                  <c:v>44641</c:v>
+                </c:pt>
+                <c:pt idx="11" c:formatCode="d\-mmm">
+                  <c:v>44642</c:v>
+                </c:pt>
+                <c:pt idx="12" c:formatCode="d\-mmm">
+                  <c:v>44643</c:v>
+                </c:pt>
+                <c:pt idx="13" c:formatCode="d\-mmm">
+                  <c:v>44644</c:v>
+                </c:pt>
+                <c:pt idx="14" c:formatCode="d\-mmm">
+                  <c:v>44645</c:v>
+                </c:pt>
+                <c:pt idx="15" c:formatCode="d\-mmm">
+                  <c:v>44646</c:v>
+                </c:pt>
+                <c:pt idx="16" c:formatCode="d\-mmm">
+                  <c:v>44647</c:v>
+                </c:pt>
+                <c:pt idx="17" c:formatCode="d\-mmm">
+                  <c:v>44648</c:v>
+                </c:pt>
+                <c:pt idx="18" c:formatCode="d\-mmm">
+                  <c:v>44649</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$2:$C$21</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$2:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>734</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>865</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>977</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>979</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2231</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2631</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3450</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4381</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5656</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum cases</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$2:$A$20</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0" c:formatCode="d\-mmm">
+                  <c:v>44631</c:v>
+                </c:pt>
+                <c:pt idx="1" c:formatCode="d\-mmm">
+                  <c:v>44632</c:v>
+                </c:pt>
+                <c:pt idx="2" c:formatCode="d\-mmm">
+                  <c:v>44633</c:v>
+                </c:pt>
+                <c:pt idx="3" c:formatCode="d\-mmm">
+                  <c:v>44634</c:v>
+                </c:pt>
+                <c:pt idx="4" c:formatCode="d\-mmm">
+                  <c:v>44635</c:v>
+                </c:pt>
+                <c:pt idx="5" c:formatCode="d\-mmm">
+                  <c:v>44636</c:v>
+                </c:pt>
+                <c:pt idx="6" c:formatCode="d\-mmm">
+                  <c:v>44637</c:v>
+                </c:pt>
+                <c:pt idx="7" c:formatCode="d\-mmm">
+                  <c:v>44638</c:v>
+                </c:pt>
+                <c:pt idx="8" c:formatCode="d\-mmm">
+                  <c:v>44639</c:v>
+                </c:pt>
+                <c:pt idx="9" c:formatCode="d\-mmm">
+                  <c:v>44640</c:v>
+                </c:pt>
+                <c:pt idx="10" c:formatCode="d\-mmm">
+                  <c:v>44641</c:v>
+                </c:pt>
+                <c:pt idx="11" c:formatCode="d\-mmm">
+                  <c:v>44642</c:v>
+                </c:pt>
+                <c:pt idx="12" c:formatCode="d\-mmm">
+                  <c:v>44643</c:v>
+                </c:pt>
+                <c:pt idx="13" c:formatCode="d\-mmm">
+                  <c:v>44644</c:v>
+                </c:pt>
+                <c:pt idx="14" c:formatCode="d\-mmm">
+                  <c:v>44645</c:v>
+                </c:pt>
+                <c:pt idx="15" c:formatCode="d\-mmm">
+                  <c:v>44646</c:v>
+                </c:pt>
+                <c:pt idx="16" c:formatCode="d\-mmm">
+                  <c:v>44647</c:v>
+                </c:pt>
+                <c:pt idx="17" c:formatCode="d\-mmm">
+                  <c:v>44648</c:v>
+                </c:pt>
+                <c:pt idx="18" c:formatCode="d\-mmm">
+                  <c:v>44649</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$D$2:$D$21</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$D$2:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>374</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>983</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1609</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2269</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2676</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4477</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5982</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="368187079"/>
+        <c:axId val="217429167"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="368187079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="217429167"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="217429167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="368187079"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-US"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>370205</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>131445</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4333875" y="133350"/>
+        <a:ext cx="5523230" cy="5427345"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -970,7 +2381,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
@@ -1248,11 +2659,35 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1"/>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>44648</v>
+      </c>
+      <c r="B19">
+        <v>96</v>
+      </c>
+      <c r="C19">
+        <v>4381</v>
+      </c>
+      <c r="D19">
+        <f>SUM(B19:C19)</f>
+        <v>4477</v>
+      </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="1"/>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>44649</v>
+      </c>
+      <c r="B20">
+        <v>326</v>
+      </c>
+      <c r="C20">
+        <v>5656</v>
+      </c>
+      <c r="D20">
+        <f>SUM(B20:C20)</f>
+        <v>5982</v>
+      </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1"/>
@@ -1260,5 +2695,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>